<commit_message>
Crisp DM lecture notes added, slide 1 finished
</commit_message>
<xml_diff>
--- a/StatisticsEssential/Module3/Investments.xlsx
+++ b/StatisticsEssential/Module3/Investments.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chiranjeev\Documents\Investment case study Cohort-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shabhushan/Desktop/projects/upgrad-ml/StatisticsEssential/Module3/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2B2613-CE67-674B-96E5-44D21166EFF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7080" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>C1</t>
   </si>
@@ -357,12 +358,18 @@
   </si>
   <si>
     <t>Sector-wise Investment Analysis</t>
+  </si>
+  <si>
+    <t>permalink</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -632,24 +639,27 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -665,13 +675,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -987,40 +994,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="3"/>
-    <col min="2" max="2" width="63.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="3"/>
+    <col min="2" max="2" width="63.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="25"/>
       <c r="C1" s="15"/>
     </row>
-    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
+    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="15"/>
     </row>
-    <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>15</v>
       </c>
@@ -1031,55 +1038,65 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>1</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="17"/>
-    </row>
-    <row r="6" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="17">
+        <v>66370</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>2</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="17"/>
-    </row>
-    <row r="7" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="17">
+        <v>66368</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>3</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="17"/>
-    </row>
-    <row r="8" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>4</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="17"/>
-    </row>
-    <row r="9" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>5</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="17"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="17">
+        <v>114954</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" s="11"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11" s="11"/>
     </row>
   </sheetData>
@@ -1102,38 +1119,38 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" customWidth="1"/>
-    <col min="2" max="2" width="53.85546875" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="2" max="2" width="53.83203125" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="23"/>
-    </row>
-    <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-    </row>
-    <row r="3" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="B1" s="27"/>
+    </row>
+    <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+    </row>
+    <row r="3" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-    </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+    </row>
+    <row r="4" spans="1:3" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
@@ -1144,7 +1161,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
         <v>1</v>
       </c>
@@ -1153,7 +1170,7 @@
       </c>
       <c r="C5" s="12"/>
     </row>
-    <row r="6" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
         <v>2</v>
       </c>
@@ -1162,7 +1179,7 @@
       </c>
       <c r="C6" s="12"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="12">
         <v>3</v>
       </c>
@@ -1171,7 +1188,7 @@
       </c>
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
         <v>4</v>
       </c>
@@ -1180,7 +1197,7 @@
       </c>
       <c r="C8" s="12"/>
     </row>
-    <row r="9" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
         <v>5</v>
       </c>
@@ -1210,38 +1227,38 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="2" max="2" width="47.1640625" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="23"/>
-    </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-    </row>
-    <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="B1" s="27"/>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+    </row>
+    <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>18</v>
       </c>
@@ -1252,7 +1269,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -1261,7 +1278,7 @@
       </c>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>2</v>
       </c>
@@ -1270,7 +1287,7 @@
       </c>
       <c r="C6" s="6"/>
     </row>
-    <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>3</v>
       </c>
@@ -1299,59 +1316,59 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="56.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="56.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="30"/>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="B1" s="31"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="24" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="19">
         <v>1</v>
       </c>
@@ -1362,7 +1379,7 @@
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="19">
         <v>2</v>
       </c>
@@ -1373,7 +1390,7 @@
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="19">
         <v>3</v>
       </c>
@@ -1384,7 +1401,7 @@
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="19">
         <v>4</v>
       </c>
@@ -1395,7 +1412,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="19">
         <v>5</v>
       </c>
@@ -1406,7 +1423,7 @@
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="19">
         <v>6</v>
       </c>
@@ -1417,7 +1434,7 @@
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="19">
         <v>7</v>
       </c>
@@ -1428,7 +1445,7 @@
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="19">
         <v>8</v>
       </c>
@@ -1439,7 +1456,7 @@
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="19">
         <v>9</v>
       </c>
@@ -1450,7 +1467,7 @@
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
     </row>
-    <row r="14" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Investment Excel - 3rd Sheet added
</commit_message>
<xml_diff>
--- a/StatisticsEssential/Module3/Investments.xlsx
+++ b/StatisticsEssential/Module3/Investments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shabhushan/Desktop/projects/upgrad-ml/StatisticsEssential/Module3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2B2613-CE67-674B-96E5-44D21166EFF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEFCDA8-DEC3-1340-A508-A25BBA0B5E35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -33,8 +33,63 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Bhushan, Shashi (US - Bengaluru)</author>
+  </authors>
+  <commentList>
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{E9343024-C33D-0643-8597-00A30E775FF6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bhushan, Shashi :</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Average: 11 Million
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">min 0.000000e+00 25% 1.600902e+06 50% 5.000000e+06 75% 1.200000e+07 max 1.760000e+10
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>C1</t>
   </si>
@@ -364,13 +419,25 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Venture</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>GBR</t>
+  </si>
+  <si>
+    <t>CHN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,6 +501,26 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -997,7 +1084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -1119,11 +1206,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1168,7 +1255,9 @@
       <c r="B5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="12">
+        <v>11748949.130000001</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
@@ -1177,7 +1266,9 @@
       <c r="B6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="12">
+        <v>958694.47</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="12">
@@ -1186,7 +1277,9 @@
       <c r="B7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="12">
+        <v>719818</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
@@ -1195,7 +1288,9 @@
       <c r="B8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="12">
+        <v>73308593.030000001</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
@@ -1204,7 +1299,9 @@
       <c r="B9" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1223,6 +1320,7 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1230,8 +1328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1276,7 +1374,9 @@
       <c r="B5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
@@ -1285,7 +1385,9 @@
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
@@ -1294,7 +1396,9 @@
       <c r="B7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
on Checkpoint 4: Sector Analysis 1
</commit_message>
<xml_diff>
--- a/StatisticsEssential/Module3/Investments.xlsx
+++ b/StatisticsEssential/Module3/Investments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shabhushan/Desktop/projects/upgrad-ml/StatisticsEssential/Module3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEFCDA8-DEC3-1340-A508-A25BBA0B5E35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2574C3F0-DBBF-3840-987C-473FF69AC3E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">min 0.000000e+00 25% 1.600902e+06 50% 5.000000e+06 75% 1.200000e+07 max 1.760000e+10
 </t>
@@ -430,7 +429,7 @@
     <t>GBR</t>
   </si>
   <si>
-    <t>CHN</t>
+    <t>IND</t>
   </si>
 </sst>
 </file>
@@ -524,7 +523,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1085,7 +1083,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1210,7 +1208,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1329,7 +1327,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Spark Funds Investment ppt
</commit_message>
<xml_diff>
--- a/StatisticsEssential/Module3/Investments.xlsx
+++ b/StatisticsEssential/Module3/Investments.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t xml:space="preserve">Table-1.1</t>
   </si>
@@ -449,7 +449,25 @@
     <t xml:space="preserve">For point 3 (top sector count-wise), which company received the highest investment?</t>
   </si>
   <si>
+    <t xml:space="preserve">Virtustream</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electric Cloud </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fresco Microchip </t>
+  </si>
+  <si>
     <t xml:space="preserve">For point 4 (second best sector count-wise), which company received the highest investment?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capella Photonics </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SenSage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ostara</t>
   </si>
 </sst>
 </file>
@@ -876,7 +894,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1005,7 +1023,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1238,7 +1256,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1423,27 +1441,39 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="28" t="n">
         <v>9</v>
       </c>
       <c r="B13" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="28" t="n">
         <v>10</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+        <v>51</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1470,7 +1500,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:E5 A6:B6 A10:E14 A8:B8 A7:C7 A9:C9">
+  <conditionalFormatting sqref="A5:E5 A6:B6 A10:E12 A8:B8 A7:C7 A9:C9 A14:E14 A13:B13 D13:E13">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -1564,6 +1594,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>